<commit_message>
Inicio do mapeamento das entidades Criação dos objetos de valor; Mappeamento da geração das entidades
</commit_message>
<xml_diff>
--- a/docs/RubricaAndamento.xlsx
+++ b/docs/RubricaAndamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\ESolucoes\FieldTech\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39F7047-7C25-4845-A341-C16A43A83FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62628AD5-E130-43E1-AC03-D731DFBDA3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="60" windowWidth="19440" windowHeight="14880" xr2:uid="{ACC2400F-1099-4EF4-9831-960274762D3C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Nº</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>Concluido</t>
+  </si>
+  <si>
+    <t>Em Andamento</t>
   </si>
 </sst>
 </file>
@@ -286,8 +289,11 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -295,11 +301,8 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -622,7 +625,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,24 +659,26 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="F2" s="5">
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -686,8 +691,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -704,8 +709,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>9</v>
@@ -716,36 +721,40 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="9">
         <v>2</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F6" s="5">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F7" s="5">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
         <v>13</v>
@@ -756,8 +765,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
         <v>14</v>
@@ -768,10 +777,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="A10" s="7">
         <v>3</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="2"/>
@@ -784,8 +793,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
         <v>17</v>
@@ -796,8 +805,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
         <v>18</v>
@@ -808,8 +817,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>19</v>
@@ -820,10 +829,10 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="9">
         <v>4</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="3"/>
@@ -836,8 +845,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
         <v>22</v>
@@ -848,8 +857,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
         <v>23</v>
@@ -860,8 +869,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
         <v>24</v>
@@ -872,10 +881,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+      <c r="A18" s="7">
         <v>5</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="2"/>
@@ -888,8 +897,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
         <v>27</v>
@@ -900,8 +909,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>28</v>
@@ -912,8 +921,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>29</v>
@@ -924,10 +933,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="A22" s="9">
         <v>6</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="3"/>
@@ -940,8 +949,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="9"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
         <v>32</v>
@@ -952,8 +961,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="9"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
         <v>33</v>
@@ -964,8 +973,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="9"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
         <v>34</v>
@@ -976,26 +985,20 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
       <c r="F26" s="6">
         <f>AVERAGE(F2:F25)</f>
-        <v>4.1666666666666664E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
     <mergeCell ref="A26:E26"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="B14:B17"/>
@@ -1003,6 +1006,12 @@
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="B22:B25"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Dtos Criação das entidades Inicio das atividades de crud
</commit_message>
<xml_diff>
--- a/docs/RubricaAndamento.xlsx
+++ b/docs/RubricaAndamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\ESolucoes\FieldTech\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62628AD5-E130-43E1-AC03-D731DFBDA3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BECA3B-5E9A-4E4B-A88D-E88999AF9025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="60" windowWidth="19440" windowHeight="14880" xr2:uid="{ACC2400F-1099-4EF4-9831-960274762D3C}"/>
+    <workbookView xWindow="5700" yWindow="0" windowWidth="21600" windowHeight="11295" xr2:uid="{ACC2400F-1099-4EF4-9831-960274762D3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Nº</t>
   </si>
@@ -149,9 +149,6 @@
     <t>Porcentagem</t>
   </si>
   <si>
-    <t>26/09/2022</t>
-  </si>
-  <si>
     <t>TOTAL CONCLUIDO</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>Em Andamento</t>
+  </si>
+  <si>
+    <t>23/09/2022</t>
   </si>
 </sst>
 </file>
@@ -624,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08164761-8E69-4F32-8694-C03A1CBCBA7B}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,10 +670,10 @@
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -684,7 +684,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F3" s="5">
         <v>1</v>
@@ -705,7 +705,7 @@
         <v>35</v>
       </c>
       <c r="I4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -715,9 +715,11 @@
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="F5" s="5">
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -732,10 +734,10 @@
         <v>11</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" s="5">
-        <v>0.05</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -746,10 +748,10 @@
         <v>12</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" s="5">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -759,9 +761,11 @@
       <c r="D8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="F8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -813,7 +817,7 @@
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="5">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -986,7 +990,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -994,7 +998,7 @@
       <c r="E26" s="11"/>
       <c r="F26" s="6">
         <f>AVERAGE(F2:F25)</f>
-        <v>6.25E-2</v>
+        <v>0.15625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Criação dos serviços para escrita e leitura da entidade técnico.
</commit_message>
<xml_diff>
--- a/docs/RubricaAndamento.xlsx
+++ b/docs/RubricaAndamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\ESolucoes\FieldTech\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BECA3B-5E9A-4E4B-A88D-E88999AF9025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3883CD-31A1-494F-B23A-B1B220261E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="0" windowWidth="21600" windowHeight="11295" xr2:uid="{ACC2400F-1099-4EF4-9831-960274762D3C}"/>
+    <workbookView xWindow="7290" yWindow="15" windowWidth="21600" windowHeight="11295" xr2:uid="{ACC2400F-1099-4EF4-9831-960274762D3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -289,11 +289,8 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -301,8 +298,11 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -624,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08164761-8E69-4F32-8694-C03A1CBCBA7B}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,10 +659,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2"/>
@@ -677,8 +677,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -691,8 +691,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -709,8 +709,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>9</v>
@@ -723,10 +723,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>2</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3"/>
@@ -741,8 +741,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
         <v>12</v>
@@ -755,8 +755,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
         <v>13</v>
@@ -769,8 +769,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
         <v>14</v>
@@ -781,10 +781,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="10">
         <v>3</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="2"/>
@@ -797,8 +797,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
         <v>17</v>
@@ -809,8 +809,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
         <v>18</v>
@@ -821,8 +821,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>19</v>
@@ -833,10 +833,10 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="8">
         <v>4</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="3"/>
@@ -849,8 +849,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
         <v>22</v>
@@ -861,8 +861,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
         <v>23</v>
@@ -873,8 +873,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
         <v>24</v>
@@ -885,10 +885,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="A18" s="10">
         <v>5</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="2"/>
@@ -901,8 +901,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
         <v>27</v>
@@ -913,8 +913,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>28</v>
@@ -925,8 +925,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>29</v>
@@ -937,10 +937,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
+      <c r="A22" s="8">
         <v>6</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="3"/>
@@ -953,8 +953,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="10"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
         <v>32</v>
@@ -965,8 +965,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="9"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
         <v>33</v>
@@ -977,8 +977,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="10"/>
+      <c r="A25" s="8"/>
+      <c r="B25" s="9"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
         <v>34</v>
@@ -989,13 +989,13 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
       <c r="F26" s="6">
         <f>AVERAGE(F2:F25)</f>
         <v>0.15625</v>
@@ -1003,6 +1003,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
     <mergeCell ref="A26:E26"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="B14:B17"/>
@@ -1010,12 +1016,6 @@
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementação dos repositorios Criação da configuração para iniciar a migração e criação do banco de dados.
</commit_message>
<xml_diff>
--- a/docs/RubricaAndamento.xlsx
+++ b/docs/RubricaAndamento.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\ESolucoes\FieldTech\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3883CD-31A1-494F-B23A-B1B220261E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3752ED3-9EE0-48C4-B165-C8F9E364FFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7290" yWindow="15" windowWidth="21600" windowHeight="11295" xr2:uid="{ACC2400F-1099-4EF4-9831-960274762D3C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ACC2400F-1099-4EF4-9831-960274762D3C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Escopo" sheetId="1" r:id="rId1"/>
+    <sheet name="RN" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Nº</t>
   </si>
@@ -289,8 +290,11 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -298,11 +302,8 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -625,7 +626,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,10 +660,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2"/>
@@ -670,15 +671,15 @@
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F2" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -691,15 +692,17 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="F4" s="5">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="H4" t="s">
         <v>35</v>
@@ -709,8 +712,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>9</v>
@@ -719,14 +722,14 @@
         <v>39</v>
       </c>
       <c r="F5" s="5">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="9">
         <v>2</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3"/>
@@ -741,8 +744,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
         <v>12</v>
@@ -755,8 +758,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
         <v>13</v>
@@ -769,8 +772,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
         <v>14</v>
@@ -781,10 +784,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="A10" s="7">
         <v>3</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="2"/>
@@ -797,8 +800,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
         <v>17</v>
@@ -809,8 +812,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
         <v>18</v>
@@ -821,8 +824,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>19</v>
@@ -833,10 +836,10 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="9">
         <v>4</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="3"/>
@@ -849,8 +852,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
         <v>22</v>
@@ -861,8 +864,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
         <v>23</v>
@@ -873,8 +876,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
         <v>24</v>
@@ -885,10 +888,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+      <c r="A18" s="7">
         <v>5</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="2"/>
@@ -901,8 +904,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
         <v>27</v>
@@ -913,8 +916,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>28</v>
@@ -925,8 +928,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>29</v>
@@ -937,10 +940,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="A22" s="9">
         <v>6</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="3"/>
@@ -953,8 +956,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="9"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
         <v>32</v>
@@ -965,8 +968,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="9"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
         <v>33</v>
@@ -977,8 +980,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="9"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
         <v>34</v>
@@ -989,26 +992,20 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
       <c r="F26" s="6">
         <f>AVERAGE(F2:F25)</f>
-        <v>0.15625</v>
+        <v>0.18124999999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
     <mergeCell ref="A26:E26"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="B14:B17"/>
@@ -1016,8 +1013,28 @@
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="B22:B25"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C57B90E-2921-48B1-983B-24F1D916F113}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Criação do Swagger Criação do CQRS Implementação do contexto para gerar a base de dados inicialmente.
</commit_message>
<xml_diff>
--- a/docs/RubricaAndamento.xlsx
+++ b/docs/RubricaAndamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\ESolucoes\FieldTech\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3752ED3-9EE0-48C4-B165-C8F9E364FFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3A6CAA-7A9E-425D-8A38-A19ED66B378A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ACC2400F-1099-4EF4-9831-960274762D3C}"/>
+    <workbookView xWindow="38280" yWindow="60" windowWidth="19440" windowHeight="14880" xr2:uid="{ACC2400F-1099-4EF4-9831-960274762D3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Escopo" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>Nº</t>
   </si>
@@ -290,11 +290,8 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -302,8 +299,11 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -626,7 +626,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,10 +660,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2"/>
@@ -678,8 +678,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -692,8 +692,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -702,7 +702,7 @@
         <v>39</v>
       </c>
       <c r="F4" s="5">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="H4" t="s">
         <v>35</v>
@@ -712,8 +712,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>9</v>
@@ -726,10 +726,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>2</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3"/>
@@ -744,8 +744,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
         <v>12</v>
@@ -758,8 +758,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
         <v>13</v>
@@ -772,36 +772,40 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="F9" s="5">
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="10">
         <v>3</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="F10" s="5">
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
         <v>17</v>
@@ -812,20 +816,22 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="F12" s="5">
         <v>0.25</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>19</v>
@@ -836,10 +842,10 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="8">
         <v>4</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="3"/>
@@ -852,8 +858,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
         <v>22</v>
@@ -864,8 +870,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
         <v>23</v>
@@ -876,8 +882,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
         <v>24</v>
@@ -888,10 +894,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="A18" s="10">
         <v>5</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="2"/>
@@ -904,8 +910,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
         <v>27</v>
@@ -916,8 +922,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>28</v>
@@ -928,8 +934,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>29</v>
@@ -940,10 +946,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
+      <c r="A22" s="8">
         <v>6</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="3"/>
@@ -956,20 +962,22 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="10"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="3"/>
+      <c r="E23" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="F23" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="9"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
         <v>33</v>
@@ -980,8 +988,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="10"/>
+      <c r="A25" s="8"/>
+      <c r="B25" s="9"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
         <v>34</v>
@@ -992,20 +1000,26 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
       <c r="F26" s="6">
         <f>AVERAGE(F2:F25)</f>
-        <v>0.18124999999999999</v>
+        <v>0.21875</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
     <mergeCell ref="A26:E26"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="B14:B17"/>
@@ -1013,12 +1027,6 @@
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Versionamento CQRS para criar técnico Mapeamento das entidades Criação da api de fornecedor Configuração da factory do contexto
</commit_message>
<xml_diff>
--- a/docs/RubricaAndamento.xlsx
+++ b/docs/RubricaAndamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\ESolucoes\FieldTech\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3A6CAA-7A9E-425D-8A38-A19ED66B378A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A989BB7B-09E3-4625-B5A7-C442C24176D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="60" windowWidth="19440" windowHeight="14880" xr2:uid="{ACC2400F-1099-4EF4-9831-960274762D3C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>Nº</t>
   </si>
@@ -290,8 +290,11 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -299,11 +302,8 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08164761-8E69-4F32-8694-C03A1CBCBA7B}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,10 +660,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2"/>
@@ -678,8 +678,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -692,8 +692,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -702,7 +702,7 @@
         <v>39</v>
       </c>
       <c r="F4" s="5">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="H4" t="s">
         <v>35</v>
@@ -712,8 +712,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>9</v>
@@ -726,10 +726,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="9">
         <v>2</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3"/>
@@ -744,8 +744,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
         <v>12</v>
@@ -758,8 +758,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
         <v>13</v>
@@ -772,8 +772,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
         <v>14</v>
@@ -786,10 +786,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="A10" s="7">
         <v>3</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="2"/>
@@ -804,20 +804,22 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="F11" s="5">
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
         <v>18</v>
@@ -830,22 +832,24 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="F13" s="5">
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="9">
         <v>4</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="3"/>
@@ -858,8 +862,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
         <v>22</v>
@@ -870,8 +874,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
         <v>23</v>
@@ -882,8 +886,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
         <v>24</v>
@@ -894,10 +898,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+      <c r="A18" s="7">
         <v>5</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="2"/>
@@ -910,8 +914,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
         <v>27</v>
@@ -922,8 +926,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>28</v>
@@ -934,8 +938,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>29</v>
@@ -946,10 +950,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="A22" s="9">
         <v>6</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="3"/>
@@ -962,8 +966,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="9"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
         <v>32</v>
@@ -976,8 +980,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="9"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
         <v>33</v>
@@ -988,8 +992,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="9"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
         <v>34</v>
@@ -1000,26 +1004,20 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
       <c r="F26" s="6">
         <f>AVERAGE(F2:F25)</f>
-        <v>0.21875</v>
+        <v>0.25208333333333338</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
     <mergeCell ref="A26:E26"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="B14:B17"/>
@@ -1027,6 +1025,12 @@
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="B22:B25"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Criação da primeira migração configuração dos profiles
</commit_message>
<xml_diff>
--- a/docs/RubricaAndamento.xlsx
+++ b/docs/RubricaAndamento.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\ESolucoes\FieldTech\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A989BB7B-09E3-4625-B5A7-C442C24176D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD2EFEC-D3F1-4008-BD11-F208A70FA371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="60" windowWidth="19440" windowHeight="14880" xr2:uid="{ACC2400F-1099-4EF4-9831-960274762D3C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="15480" xr2:uid="{ACC2400F-1099-4EF4-9831-960274762D3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Escopo" sheetId="1" r:id="rId1"/>
     <sheet name="RN" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>Nº</t>
   </si>
@@ -290,11 +291,8 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -302,8 +300,11 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -626,7 +627,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,10 +661,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2"/>
@@ -678,8 +679,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -692,8 +693,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -712,8 +713,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>9</v>
@@ -726,10 +727,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>2</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3"/>
@@ -744,8 +745,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
         <v>12</v>
@@ -754,26 +755,26 @@
         <v>39</v>
       </c>
       <c r="F7" s="5">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F8" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
         <v>14</v>
@@ -786,10 +787,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="10">
         <v>3</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="2"/>
@@ -804,8 +805,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
         <v>17</v>
@@ -818,8 +819,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
         <v>18</v>
@@ -832,8 +833,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>19</v>
@@ -846,10 +847,10 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="8">
         <v>4</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="3"/>
@@ -862,8 +863,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
         <v>22</v>
@@ -874,8 +875,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
         <v>23</v>
@@ -886,8 +887,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
         <v>24</v>
@@ -898,10 +899,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="A18" s="10">
         <v>5</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="2"/>
@@ -914,8 +915,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
         <v>27</v>
@@ -926,8 +927,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>28</v>
@@ -938,8 +939,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>29</v>
@@ -950,10 +951,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
+      <c r="A22" s="8">
         <v>6</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="3"/>
@@ -966,22 +967,22 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="10"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F23" s="5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="9"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
         <v>33</v>
@@ -992,32 +993,40 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="10"/>
+      <c r="A25" s="8"/>
+      <c r="B25" s="9"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="3"/>
+      <c r="E25" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="F25" s="5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
       <c r="F26" s="6">
         <f>AVERAGE(F2:F25)</f>
-        <v>0.25208333333333338</v>
+        <v>0.28750000000000003</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
     <mergeCell ref="A26:E26"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="B14:B17"/>
@@ -1025,12 +1034,6 @@
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Criação do CQRS do fornecedor para incluir e carregar todos Criação dos serviços
</commit_message>
<xml_diff>
--- a/docs/RubricaAndamento.xlsx
+++ b/docs/RubricaAndamento.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\ESolucoes\FieldTech\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD2EFEC-D3F1-4008-BD11-F208A70FA371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6548A188-1E43-4B31-A8B3-64733A424747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="15480" xr2:uid="{ACC2400F-1099-4EF4-9831-960274762D3C}"/>
+    <workbookView xWindow="57480" yWindow="-855" windowWidth="29040" windowHeight="15720" xr2:uid="{ACC2400F-1099-4EF4-9831-960274762D3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Escopo" sheetId="1" r:id="rId1"/>
     <sheet name="RN" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -291,8 +290,11 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -300,11 +302,8 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -627,7 +626,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,10 +660,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2"/>
@@ -679,8 +678,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -693,8 +692,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -713,8 +712,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>9</v>
@@ -723,14 +722,14 @@
         <v>39</v>
       </c>
       <c r="F5" s="5">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="9">
         <v>2</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3"/>
@@ -745,8 +744,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
         <v>12</v>
@@ -759,8 +758,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
         <v>13</v>
@@ -773,8 +772,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
         <v>14</v>
@@ -787,10 +786,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="A10" s="7">
         <v>3</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="2"/>
@@ -805,8 +804,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
         <v>17</v>
@@ -819,8 +818,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
         <v>18</v>
@@ -833,8 +832,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>19</v>
@@ -847,10 +846,10 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="9">
         <v>4</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="3"/>
@@ -863,8 +862,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
         <v>22</v>
@@ -875,8 +874,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
         <v>23</v>
@@ -887,8 +886,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
         <v>24</v>
@@ -899,10 +898,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+      <c r="A18" s="7">
         <v>5</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="2"/>
@@ -915,8 +914,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
         <v>27</v>
@@ -927,8 +926,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>28</v>
@@ -939,8 +938,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>29</v>
@@ -951,10 +950,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="A22" s="9">
         <v>6</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="3"/>
@@ -967,8 +966,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="9"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
         <v>32</v>
@@ -981,8 +980,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="9"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
         <v>33</v>
@@ -993,8 +992,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="9"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
         <v>34</v>
@@ -1007,26 +1006,20 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
       <c r="F26" s="6">
         <f>AVERAGE(F2:F25)</f>
-        <v>0.28750000000000003</v>
+        <v>0.30000000000000004</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
     <mergeCell ref="A26:E26"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="B14:B17"/>
@@ -1034,6 +1027,12 @@
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="B22:B25"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementação dos dtos Entidades e ajustes para gravar as ordem de serviço
</commit_message>
<xml_diff>
--- a/docs/RubricaAndamento.xlsx
+++ b/docs/RubricaAndamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\ESolucoes\FieldTech\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6548A188-1E43-4B31-A8B3-64733A424747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3B899F-1F42-4383-BAF1-04B564D5E062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-855" windowWidth="29040" windowHeight="15720" xr2:uid="{ACC2400F-1099-4EF4-9831-960274762D3C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="15480" xr2:uid="{ACC2400F-1099-4EF4-9831-960274762D3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Escopo" sheetId="1" r:id="rId1"/>
@@ -290,11 +290,8 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -302,8 +299,11 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08164761-8E69-4F32-8694-C03A1CBCBA7B}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,10 +660,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2"/>
@@ -678,8 +678,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -692,8 +692,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -702,7 +702,7 @@
         <v>39</v>
       </c>
       <c r="F4" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="H4" t="s">
         <v>35</v>
@@ -712,8 +712,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>9</v>
@@ -726,10 +726,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>2</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3"/>
@@ -740,12 +740,12 @@
         <v>39</v>
       </c>
       <c r="F6" s="5">
-        <v>0.35</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
         <v>12</v>
@@ -754,12 +754,12 @@
         <v>39</v>
       </c>
       <c r="F7" s="5">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
         <v>13</v>
@@ -772,8 +772,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
         <v>14</v>
@@ -782,14 +782,14 @@
         <v>39</v>
       </c>
       <c r="F9" s="5">
-        <v>0.15</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="10">
         <v>3</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="2"/>
@@ -800,12 +800,12 @@
         <v>39</v>
       </c>
       <c r="F10" s="5">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
         <v>17</v>
@@ -814,12 +814,12 @@
         <v>39</v>
       </c>
       <c r="F11" s="5">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
         <v>18</v>
@@ -828,12 +828,12 @@
         <v>39</v>
       </c>
       <c r="F12" s="5">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>19</v>
@@ -846,10 +846,10 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="8">
         <v>4</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="3"/>
@@ -862,8 +862,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
         <v>22</v>
@@ -874,8 +874,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
         <v>23</v>
@@ -886,22 +886,22 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="A18" s="10">
         <v>5</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="2"/>
@@ -914,20 +914,20 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>28</v>
@@ -938,8 +938,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>29</v>
@@ -950,10 +950,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
+      <c r="A22" s="8">
         <v>6</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="3"/>
@@ -966,8 +966,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="10"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
         <v>32</v>
@@ -980,8 +980,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="9"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
         <v>33</v>
@@ -992,8 +992,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="10"/>
+      <c r="A25" s="8"/>
+      <c r="B25" s="9"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
         <v>34</v>
@@ -1006,20 +1006,26 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
       <c r="F26" s="6">
         <f>AVERAGE(F2:F25)</f>
-        <v>0.30000000000000004</v>
+        <v>0.44208333333333338</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
     <mergeCell ref="A26:E26"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="B14:B17"/>
@@ -1027,12 +1033,6 @@
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Correção dos objetos que estavam incorretos Correção dos profiles Ajuste na execução do mapping campos truncados.
</commit_message>
<xml_diff>
--- a/docs/RubricaAndamento.xlsx
+++ b/docs/RubricaAndamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\ESolucoes\FieldTech\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3B899F-1F42-4383-BAF1-04B564D5E062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6355D140-B5E9-41D8-AC39-B4623FF20232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="15480" xr2:uid="{ACC2400F-1099-4EF4-9831-960274762D3C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ACC2400F-1099-4EF4-9831-960274762D3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Escopo" sheetId="1" r:id="rId1"/>
@@ -290,8 +290,11 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -299,11 +302,8 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -626,7 +626,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,10 +660,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2"/>
@@ -678,8 +678,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -692,8 +692,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -712,8 +712,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>9</v>
@@ -722,14 +722,14 @@
         <v>39</v>
       </c>
       <c r="F5" s="5">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="9">
         <v>2</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3"/>
@@ -744,22 +744,22 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F7" s="5">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
         <v>13</v>
@@ -772,8 +772,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
         <v>14</v>
@@ -786,10 +786,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="A10" s="7">
         <v>3</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="2"/>
@@ -800,12 +800,12 @@
         <v>39</v>
       </c>
       <c r="F10" s="5">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
         <v>17</v>
@@ -814,12 +814,12 @@
         <v>39</v>
       </c>
       <c r="F11" s="5">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
         <v>18</v>
@@ -832,8 +832,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>19</v>
@@ -846,10 +846,10 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="9">
         <v>4</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="3"/>
@@ -862,8 +862,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
         <v>22</v>
@@ -874,8 +874,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
         <v>23</v>
@@ -886,8 +886,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
         <v>24</v>
@@ -898,10 +898,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+      <c r="A18" s="7">
         <v>5</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="2"/>
@@ -914,8 +914,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
         <v>27</v>
@@ -926,8 +926,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>28</v>
@@ -938,8 +938,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>29</v>
@@ -950,10 +950,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="A22" s="9">
         <v>6</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="3"/>
@@ -966,8 +966,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="9"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
         <v>32</v>
@@ -980,8 +980,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="9"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
         <v>33</v>
@@ -992,8 +992,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="9"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
         <v>34</v>
@@ -1006,26 +1006,20 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
       <c r="F26" s="6">
         <f>AVERAGE(F2:F25)</f>
-        <v>0.44208333333333338</v>
+        <v>0.47958333333333331</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
     <mergeCell ref="A26:E26"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="B14:B17"/>
@@ -1033,6 +1027,12 @@
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="B22:B25"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Registrando configurações de ambiente de deploy
</commit_message>
<xml_diff>
--- a/docs/RubricaAndamento.xlsx
+++ b/docs/RubricaAndamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\ESolucoes\FieldTech\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A39BC4-4E14-488E-AB76-0CE4FC52383B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22E75C8-FF6F-411D-8069-100BF6C2EEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ACC2400F-1099-4EF4-9831-960274762D3C}"/>
+    <workbookView xWindow="19590" yWindow="0" windowWidth="18810" windowHeight="15480" xr2:uid="{ACC2400F-1099-4EF4-9831-960274762D3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Escopo" sheetId="1" r:id="rId1"/>
@@ -290,8 +290,11 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -299,11 +302,8 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08164761-8E69-4F32-8694-C03A1CBCBA7B}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,10 +660,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <v>1</v>
-      </c>
-      <c r="B2" s="11" t="s">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2"/>
@@ -678,8 +678,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -692,8 +692,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -712,8 +712,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>9</v>
@@ -726,10 +726,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="9">
         <v>2</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3"/>
@@ -744,8 +744,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
         <v>12</v>
@@ -758,8 +758,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
         <v>13</v>
@@ -772,8 +772,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
         <v>14</v>
@@ -786,10 +786,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="A10" s="7">
         <v>3</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="2"/>
@@ -800,12 +800,12 @@
         <v>39</v>
       </c>
       <c r="F10" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
         <v>17</v>
@@ -814,12 +814,12 @@
         <v>39</v>
       </c>
       <c r="F11" s="5">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
         <v>18</v>
@@ -832,8 +832,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>19</v>
@@ -846,10 +846,10 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="9">
         <v>4</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="3"/>
@@ -858,12 +858,12 @@
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
         <v>22</v>
@@ -874,8 +874,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
         <v>23</v>
@@ -886,8 +886,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
         <v>24</v>
@@ -898,10 +898,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+      <c r="A18" s="7">
         <v>5</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="2"/>
@@ -910,12 +910,12 @@
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
         <v>27</v>
@@ -926,34 +926,34 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="A22" s="9">
         <v>6</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="3"/>
@@ -962,12 +962,12 @@
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="9"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
         <v>32</v>
@@ -980,8 +980,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="9"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
         <v>33</v>
@@ -992,8 +992,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="9"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
         <v>34</v>
@@ -1002,30 +1002,24 @@
         <v>39</v>
       </c>
       <c r="F25" s="5">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
       <c r="F26" s="6">
         <f>AVERAGE(F2:F25)</f>
-        <v>0.60208333333333341</v>
+        <v>0.86458333333333337</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
     <mergeCell ref="A26:E26"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="B14:B17"/>
@@ -1033,6 +1027,12 @@
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="B22:B25"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ajustes do projeto para executar local.
</commit_message>
<xml_diff>
--- a/docs/RubricaAndamento.xlsx
+++ b/docs/RubricaAndamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\ESolucoes\FieldTech\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22E75C8-FF6F-411D-8069-100BF6C2EEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C408D84C-6A9D-4BC8-9DE2-E86BDF9C305E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19590" yWindow="0" windowWidth="18810" windowHeight="15480" xr2:uid="{ACC2400F-1099-4EF4-9831-960274762D3C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ACC2400F-1099-4EF4-9831-960274762D3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Escopo" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
   <si>
     <t>Nº</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>23/09/2022</t>
+  </si>
+  <si>
+    <t>Não feito</t>
   </si>
 </sst>
 </file>
@@ -290,11 +293,8 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -302,8 +302,11 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -626,7 +629,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,10 +663,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2"/>
@@ -678,8 +681,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -692,8 +695,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -712,8 +715,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>9</v>
@@ -726,10 +729,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>2</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3"/>
@@ -737,15 +740,15 @@
         <v>11</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F6" s="5">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
         <v>12</v>
@@ -758,8 +761,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
         <v>13</v>
@@ -772,24 +775,24 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="10">
         <v>3</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="2"/>
@@ -797,177 +800,195 @@
         <v>16</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F11" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F13" s="5">
-        <v>0.15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="8">
         <v>4</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="F14" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="F15" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="F16" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="F17" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="A18" s="10">
         <v>5</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="F18" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="F19" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="F20" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="F21" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
+      <c r="A22" s="8">
         <v>6</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="F22" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="10"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
         <v>32</v>
@@ -980,46 +1001,54 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="9"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="3"/>
+      <c r="E24" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="F24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="10"/>
+      <c r="A25" s="8"/>
+      <c r="B25" s="9"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F25" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
       <c r="F26" s="6">
         <f>AVERAGE(F2:F25)</f>
-        <v>0.86458333333333337</v>
+        <v>0.95833333333333337</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
     <mergeCell ref="A26:E26"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="B14:B17"/>
@@ -1027,12 +1056,6 @@
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>